<commit_message>
boilerplate visuals, expanded boilerplate dictionary
</commit_message>
<xml_diff>
--- a/data_sample.xlsx
+++ b/data_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarus\OneDrive\Desktop\TUM\5. Sem\SEM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarus\OneDrive\Desktop\TUM\5. Sem\SEM\sec-cyber-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79723DFC-5D2B-4CCA-90D0-1D3B9506D2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D3B6D8-7B18-44B7-8816-9C83DBE36456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5E450EC3-0B73-40DF-881C-3824894009BE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="146">
   <si>
     <t>ticker</t>
   </si>
@@ -74,12 +74,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>LLY</t>
   </si>
   <si>
@@ -122,12 +116,6 @@
     <t>Visa Inc.</t>
   </si>
   <si>
-    <t>Tesla, Inc.</t>
-  </si>
-  <si>
-    <t>Ford Motor Company</t>
-  </si>
-  <si>
     <t>Johnson &amp; Johnson</t>
   </si>
   <si>
@@ -155,9 +143,6 @@
     <t>Finance</t>
   </si>
   <si>
-    <t>Automotive</t>
-  </si>
-  <si>
     <t>Healthcare</t>
   </si>
   <si>
@@ -417,12 +402,6 @@
   </si>
   <si>
     <t>1.409B</t>
-  </si>
-  <si>
-    <t>1.535T</t>
-  </si>
-  <si>
-    <t>54.975B</t>
   </si>
   <si>
     <t>595.0B</t>
@@ -624,8 +603,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}" name="Tabelle1" displayName="Tabelle1" ref="A1:I44" totalsRowShown="0">
-  <autoFilter ref="A1:I44" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}" name="Tabelle1" displayName="Tabelle1" ref="A1:I42" totalsRowShown="0">
+  <autoFilter ref="A1:I42" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5769C743-18AD-4052-A3FE-AC057354AA2B}" name="ticker"/>
     <tableColumn id="2" xr3:uid="{A21D783E-B619-4DF5-925A-7B6F310BCCFD}" name="company"/>
@@ -958,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BFCDBB-FBE1-4A3C-9FDE-7149507C4FC1}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,28 +965,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="I1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1015,32 +994,32 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K2">
         <f>COUNTIF($D:$D, "Large")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2">
         <f>COUNTIF($D:$D, "Medium")</f>
@@ -1056,28 +1035,28 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -1085,144 +1064,144 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -1230,28 +1209,28 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -1259,144 +1238,144 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -1404,28 +1383,28 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -1433,144 +1412,144 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1578,695 +1557,637 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
         <v>40</v>
       </c>
-      <c r="D30" t="s">
-        <v>44</v>
-      </c>
       <c r="E30" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
         <v>40</v>
       </c>
-      <c r="D31" t="s">
-        <v>44</v>
-      </c>
       <c r="E31" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>150</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
content scoring and new length_visuals
</commit_message>
<xml_diff>
--- a/data_sample.xlsx
+++ b/data_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarus\OneDrive\Desktop\TUM\5. Sem\SEM\sec-cyber-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D3B6D8-7B18-44B7-8816-9C83DBE36456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8179982-6FD9-429C-AAF7-AA8886BAC596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5E450EC3-0B73-40DF-881C-3824894009BE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="147">
   <si>
     <t>ticker</t>
   </si>
@@ -161,15 +161,6 @@
     <t>Small</t>
   </si>
   <si>
-    <t>large count</t>
-  </si>
-  <si>
-    <t>medium count</t>
-  </si>
-  <si>
-    <t>small count</t>
-  </si>
-  <si>
     <t>NKE</t>
   </si>
   <si>
@@ -474,6 +465,18 @@
   </si>
   <si>
     <t>458.3M</t>
+  </si>
+  <si>
+    <t>C_2022</t>
+  </si>
+  <si>
+    <t>C_2023</t>
+  </si>
+  <si>
+    <t>C_2024</t>
+  </si>
+  <si>
+    <t>C_2025</t>
   </si>
 </sst>
 </file>
@@ -603,9 +606,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}" name="Tabelle1" displayName="Tabelle1" ref="A1:I42" totalsRowShown="0">
-  <autoFilter ref="A1:I42" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}" name="Tabelle1" displayName="Tabelle1" ref="A1:M42" totalsRowShown="0">
+  <autoFilter ref="A1:M42" xr:uid="{E5D2933D-2376-4D9B-B83A-CA6AC384A388}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{5769C743-18AD-4052-A3FE-AC057354AA2B}" name="ticker"/>
     <tableColumn id="2" xr3:uid="{A21D783E-B619-4DF5-925A-7B6F310BCCFD}" name="company"/>
     <tableColumn id="3" xr3:uid="{52D0AEAC-68CC-49D8-B682-B39258443DC5}" name="industry"/>
@@ -615,6 +618,10 @@
     <tableColumn id="7" xr3:uid="{76B39A2F-86C8-4C80-9D6D-82034FEAD36A}" name="2023" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{B14E79DC-7277-4671-928D-E33610613A3D}" name="2024" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{E917151E-5942-4C59-8443-F783F48B84C5}" name="2025" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{74FBFD9B-117D-494B-9634-21D0DA99ABE8}" name="C_2022"/>
+    <tableColumn id="11" xr3:uid="{34BA3B9F-2838-47A4-9A1A-59952999AEC5}" name="C_2023"/>
+    <tableColumn id="12" xr3:uid="{92BBEED1-C805-4B4A-9960-EB1F479CE836}" name="C_2024"/>
+    <tableColumn id="13" xr3:uid="{F2F8E8BF-C592-428C-ACE6-FC479FE65E85}" name="C_2025"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -939,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BFCDBB-FBE1-4A3C-9FDE-7149507C4FC1}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -965,28 +972,31 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" t="s">
         <v>139</v>
       </c>
-      <c r="G1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" t="s">
-        <v>142</v>
+      <c r="J1" t="s">
+        <v>143</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>144</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>145</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1003,31 +1013,31 @@
         <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2">
-        <f>COUNTIF($D:$D, "Large")</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <f>COUNTIF($D:$D, "Medium")</f>
-        <v>14</v>
+        <v>0.17</v>
       </c>
       <c r="M2">
-        <f>COUNTIF($D:$D,"Small")</f>
-        <v>14</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1044,19 +1054,31 @@
         <v>38</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0.33</v>
+      </c>
+      <c r="L3">
+        <v>0.33</v>
+      </c>
+      <c r="M3">
+        <v>0.33</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -1073,27 +1095,39 @@
         <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J4">
+        <v>0.33</v>
+      </c>
+      <c r="K4">
+        <v>0.33</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -1102,27 +1136,39 @@
         <v>39</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0.67</v>
+      </c>
+      <c r="L5">
+        <v>0.67</v>
+      </c>
+      <c r="M5">
+        <v>0.67</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -1131,19 +1177,31 @@
         <v>39</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J6">
+        <v>0.17</v>
+      </c>
+      <c r="K6">
+        <v>0.17</v>
+      </c>
+      <c r="L6">
+        <v>0.33</v>
+      </c>
+      <c r="M6">
+        <v>0.83</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -1160,27 +1218,39 @@
         <v>40</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0.33</v>
+      </c>
+      <c r="L7">
+        <v>0.83</v>
+      </c>
+      <c r="M7">
+        <v>0.83</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
@@ -1189,19 +1259,31 @@
         <v>40</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0.33</v>
+      </c>
+      <c r="L8">
+        <v>0.33</v>
+      </c>
+      <c r="M8">
+        <v>0.33</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -1218,19 +1300,31 @@
         <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0.33</v>
+      </c>
+      <c r="L9">
+        <v>0.5</v>
+      </c>
+      <c r="M9">
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -1247,27 +1341,39 @@
         <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J10">
+        <v>0.17</v>
+      </c>
+      <c r="K10">
+        <v>0.33</v>
+      </c>
+      <c r="L10">
+        <v>0.17</v>
+      </c>
+      <c r="M10">
+        <v>0.17</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -1276,27 +1382,39 @@
         <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0.33</v>
+      </c>
+      <c r="L11">
+        <v>0.33</v>
+      </c>
+      <c r="M11">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
@@ -1305,27 +1423,39 @@
         <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.33</v>
+      </c>
+      <c r="M12">
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>32</v>
@@ -1334,27 +1464,39 @@
         <v>40</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0.33</v>
+      </c>
+      <c r="L13">
+        <v>0.67</v>
+      </c>
+      <c r="M13">
+        <v>0.67</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1363,19 +1505,31 @@
         <v>40</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0.17</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -1392,19 +1546,31 @@
         <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -1421,27 +1587,39 @@
         <v>38</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J16">
+        <v>0.17</v>
+      </c>
+      <c r="K16">
+        <v>0.17</v>
+      </c>
+      <c r="L16">
+        <v>0.5</v>
+      </c>
+      <c r="M16">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -1450,27 +1628,39 @@
         <v>39</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17">
+        <v>0.17</v>
+      </c>
+      <c r="K17">
+        <v>0.17</v>
+      </c>
+      <c r="L17">
+        <v>0.67</v>
+      </c>
+      <c r="M17">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>69</v>
-      </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
@@ -1479,27 +1669,39 @@
         <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J18">
+        <v>0.17</v>
+      </c>
+      <c r="K18">
+        <v>0.67</v>
+      </c>
+      <c r="L18">
+        <v>0.67</v>
+      </c>
+      <c r="M18">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
@@ -1508,27 +1710,39 @@
         <v>40</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J19">
+        <v>0.17</v>
+      </c>
+      <c r="K19">
+        <v>0.17</v>
+      </c>
+      <c r="L19">
+        <v>0.67</v>
+      </c>
+      <c r="M19">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -1537,22 +1751,34 @@
         <v>40</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J20">
+        <v>0.33</v>
+      </c>
+      <c r="K20">
+        <v>0.86</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1566,27 +1792,39 @@
         <v>38</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J21">
+        <v>0.17</v>
+      </c>
+      <c r="K21">
+        <v>0.17</v>
+      </c>
+      <c r="L21">
+        <v>0.83</v>
+      </c>
+      <c r="M21">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -1595,27 +1833,39 @@
         <v>39</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J22">
+        <v>0.17</v>
+      </c>
+      <c r="K22">
+        <v>0.17</v>
+      </c>
+      <c r="L22">
+        <v>0.83</v>
+      </c>
+      <c r="M22">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -1624,27 +1874,39 @@
         <v>39</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0.67</v>
+      </c>
+      <c r="M23">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -1653,27 +1915,39 @@
         <v>40</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0.67</v>
+      </c>
+      <c r="L24">
+        <v>0.67</v>
+      </c>
+      <c r="M24">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" t="s">
         <v>117</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" t="s">
-        <v>120</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -1682,22 +1956,34 @@
         <v>40</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0.33</v>
+      </c>
+      <c r="M25">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1711,27 +1997,39 @@
         <v>38</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0.33</v>
+      </c>
+      <c r="L26">
+        <v>0.33</v>
+      </c>
+      <c r="M26">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1740,27 +2038,39 @@
         <v>38</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0.33</v>
+      </c>
+      <c r="L27">
+        <v>0.5</v>
+      </c>
+      <c r="M27">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
@@ -1769,27 +2079,39 @@
         <v>39</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0.5</v>
+      </c>
+      <c r="L28">
+        <v>0.5</v>
+      </c>
+      <c r="M28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
@@ -1798,27 +2120,39 @@
         <v>39</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0.67</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
@@ -1827,27 +2161,39 @@
         <v>40</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0.5</v>
+      </c>
+      <c r="M30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -1856,22 +2202,34 @@
         <v>40</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0.17</v>
+      </c>
+      <c r="M31">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1885,27 +2243,39 @@
         <v>38</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J32">
+        <v>0.17</v>
+      </c>
+      <c r="K32">
+        <v>0.33</v>
+      </c>
+      <c r="L32">
+        <v>0.33</v>
+      </c>
+      <c r="M32">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
@@ -1914,27 +2284,39 @@
         <v>39</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0.5</v>
+      </c>
+      <c r="L33">
+        <v>0.67</v>
+      </c>
+      <c r="M33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>36</v>
@@ -1943,27 +2325,39 @@
         <v>39</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0.33</v>
+      </c>
+      <c r="M34">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
@@ -1972,27 +2366,39 @@
         <v>40</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0.5</v>
+      </c>
+      <c r="L35">
+        <v>0.5</v>
+      </c>
+      <c r="M35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
         <v>36</v>
@@ -2001,27 +2407,39 @@
         <v>40</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0.5</v>
+      </c>
+      <c r="M36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
@@ -2030,27 +2448,39 @@
         <v>38</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0.5</v>
+      </c>
+      <c r="L37">
+        <v>0.5</v>
+      </c>
+      <c r="M37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
@@ -2059,22 +2489,34 @@
         <v>38</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0.67</v>
+      </c>
+      <c r="M38">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2088,22 +2530,34 @@
         <v>39</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0.5</v>
+      </c>
+      <c r="L39">
+        <v>0.5</v>
+      </c>
+      <c r="M39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2117,27 +2571,39 @@
         <v>39</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0.5</v>
+      </c>
+      <c r="M40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
         <v>37</v>
@@ -2146,27 +2612,39 @@
         <v>40</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0.5</v>
+      </c>
+      <c r="M41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
@@ -2175,19 +2653,31 @@
         <v>40</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0.67</v>
+      </c>
+      <c r="M42">
+        <v>0.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>